<commit_message>
Se agrega nuevo caso de prueba
</commit_message>
<xml_diff>
--- a/Rol Tercero/Sumario.xlsx
+++ b/Rol Tercero/Sumario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Prueba\Rol Tercero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9542FD6-9595-4E93-8B8F-6354424277F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682B8568-1DD6-4A52-93C4-6AD327233572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>N°</t>
   </si>
@@ -39,15 +39,9 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>CP_002</t>
-  </si>
-  <si>
     <t>Registrar un cliente con todos los campos en blanco menos el telefono que</t>
   </si>
   <si>
-    <t>Prueba de validacion campos numericos en firstname</t>
-  </si>
-  <si>
     <t>CP_003</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>Registra un cliente con todos los campos en blanco</t>
   </si>
   <si>
-    <t>Reportado</t>
-  </si>
-  <si>
     <t>Abierto</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
     <t>Prioridad</t>
   </si>
   <si>
-    <t>media</t>
-  </si>
-  <si>
     <t>baja</t>
   </si>
   <si>
@@ -94,6 +82,15 @@
   </si>
   <si>
     <t>aprovado</t>
+  </si>
+  <si>
+    <t>CP_lista_campos_registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como se aprecia en la imagen X, la lista no trae informacion y al ser un campo obligatorio no puese realizar la accion </t>
+  </si>
+  <si>
+    <t>alta</t>
   </si>
 </sst>
 </file>
@@ -380,62 +377,62 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,7 +717,7 @@
   <dimension ref="B2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H8"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,149 +731,164 @@
   <sheetData>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="9"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="7"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="2:11" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="18"/>
+      <c r="C5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="2:11" ht="47.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="20"/>
+      <c r="C6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="2:11" ht="47.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="19" t="s">
+      <c r="C7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="2:11" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="20"/>
+      <c r="C8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="12"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" spans="2:11" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
+      <c r="C9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="G3:H4"/>
     <mergeCell ref="G5:H5"/>
@@ -890,19 +902,6 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>